<commit_message>
UPdated kri for september month end 2024
</commit_message>
<xml_diff>
--- a/Data/20240802_KRI_Report_New.xlsx
+++ b/Data/20240802_KRI_Report_New.xlsx
@@ -13,14 +13,15 @@
     <sheet name="April2024" sheetId="4" r:id="rId4"/>
     <sheet name="May2024" sheetId="5" r:id="rId5"/>
     <sheet name="June2024" sheetId="6" r:id="rId6"/>
-    <sheet name="July2024" sheetId="7" r:id="rId7"/>
+    <sheet name="JuLy2024" sheetId="7" r:id="rId7"/>
+    <sheet name="August2024" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="9">
   <si>
     <t>new_loan_type</t>
   </si>
@@ -1065,4 +1066,99 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>0.504</v>
+      </c>
+      <c r="C2">
+        <v>32.806</v>
+      </c>
+      <c r="D2">
+        <v>28.201</v>
+      </c>
+      <c r="E2">
+        <v>24.029</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>9.507999999999999</v>
+      </c>
+      <c r="C3">
+        <v>38.088</v>
+      </c>
+      <c r="D3">
+        <v>30.153</v>
+      </c>
+      <c r="E3">
+        <v>35.92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>6.25</v>
+      </c>
+      <c r="C4">
+        <v>21.766</v>
+      </c>
+      <c r="D4">
+        <v>15.63</v>
+      </c>
+      <c r="E4">
+        <v>18.821</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>23.937</v>
+      </c>
+      <c r="D5">
+        <v>17.631</v>
+      </c>
+      <c r="E5">
+        <v>21.193</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>